<commit_message>
Updated Arbeitspaketplanung according to new Gantt
</commit_message>
<xml_diff>
--- a/KanBan-App/Documents/Zeitmanagement/Arbeitspaketbeschreibungen_als_Excel.xlsx
+++ b/KanBan-App/Documents/Zeitmanagement/Arbeitspaketbeschreibungen_als_Excel.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="102">
   <si>
     <t>Vorgangsname</t>
   </si>
@@ -253,13 +253,85 @@
   </si>
   <si>
     <t>Arbeitspaketbeschreibung</t>
+  </si>
+  <si>
+    <t>Hierbei handelt es sich um eine Unterrichtseinheit bei Hr. Yass</t>
+  </si>
+  <si>
+    <t>Hierbei handelte es sich um eine Unterrichtseinheit bei Hr. Yass - Nach dem Umplanung wurde diese Einheit freigegeben</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Die Vorgaben des Unterrichts werden besprochen aber abgewogen. Am Ende entscheidet man sich für einen Vorschlag (KanKan-Board oder Scrum-Lernprogramm)</t>
+  </si>
+  <si>
+    <t>Nachdem entschieden wurde welches Projekt umgesetzt wird müssen nun Ideen für das Projekt gesammelt werden. Jeder Projektmitarbeiter entwickelt eigenständig Idee über die mögliche Umsetzung der Software</t>
+  </si>
+  <si>
+    <t>Die gesammelten Ideen der einzelnen Projektmitarbeiten müssen in diesem Arbeitspaket besprochen und bewertet werden. Mindestanforderungen und mögliche Optionale Ergänzungen werden diskutiert und bewertet um diese anschließend in der Projektdefinition festzuhalten.</t>
+  </si>
+  <si>
+    <t>Da wird uns für das KanBan-Board entschieden haben muss nun über KanBan recherchiert werden. Ebenso werden bereits vorhandene ähnlich Apps im Store angesehen und analysiert. (Beispielsweise "KanBanBoard" von "giApps")</t>
+  </si>
+  <si>
+    <t>In diesem Arbeitspaket muss über das Frontend-Framework Universal Windows Platform recherchiert werden. Mögliche Designpatterns werden analysiert und im Team besprochen.</t>
+  </si>
+  <si>
+    <t>In diesem Arbeitspaket muss über die relativ neue Technologie .NET Core, eine modulare Abwandlung des .NET Frameworks, recherchiert werden. Design-Patterns und Technologie wie das EntityFramework müssen angesehen und deren mögliche Verwendung bewertet werden.</t>
+  </si>
+  <si>
+    <t>Als Persistenzschicht wurde SQLite ausgewählt, eine Datenbank die auch speziell in mobilen Frontend Anwendungen häufig eingesetzt wird. Die Ansteuerung über das .NET Core Backend muss analysiert und bewertet werden.</t>
+  </si>
+  <si>
+    <t>Hierbei handelt es sich um ein Teammeeting. Zum Abschluss des Meetings wird ein Protokoll erstellt.</t>
+  </si>
+  <si>
+    <t>Der Projektstrukturplan muss erstellt werden. Hierfür wird MS-Projekt eingesetzt. Der PSP wird im Laufe der Projektes noch weiter entwickelt und eventuell umgestaltet.</t>
+  </si>
+  <si>
+    <t>Die Arbeitpakete müssen beschrieben werde, sodass jeder Mitarbeiter genau weis, was zu tun ist wenn ihm ein Arbeitspaket zugeordnet wird.</t>
+  </si>
+  <si>
+    <t>Ein extra Zeitplan in Excelform muss erstellt werden, in welche die Teammitglieder ihre investierten Stunden eintragen können.</t>
+  </si>
+  <si>
+    <t>Die Projektdefinition muss geschrieben werden. Hier werden Zielgruppe, Technologien und Kernfeatures festgehalten. Ebenso werden einige Optionale Features beschrieben.</t>
+  </si>
+  <si>
+    <t>Die in der Projektdefinition festgelegten Hauptfeatures des Programms sollen mit Programmablaufdiagrammen beschrieben werden.</t>
+  </si>
+  <si>
+    <t>Das zugrunde liegende Datenmodell muss in diesem Arbeitspaket festgelegt werden. Hierzu soll ein UML oder Entity Diagramm verwendet werden.</t>
+  </si>
+  <si>
+    <t>Simple Codestandards werden festgelegt und beschrieben.</t>
+  </si>
+  <si>
+    <t>Die zu verwendenden Technologien müssen festegelegt werden. Hier zählen auch Nuget Packages von denen bereits bekannt ist, dass sie verwendet werden und etwaige Zusatzsoftware dazu.</t>
+  </si>
+  <si>
+    <t>Das vorher festgelegte Datenmodell muss in diesem Arbeitspaket als SQLite Datenbank umgesetzt werden. Auf Beziehungen zwischen den Entitäten ist zu achten.</t>
+  </si>
+  <si>
+    <t>Die erstellte Datenbank muss per Entity-Framework (Entity-Relationship-Mapper) mit dem Backend verknüpft werden. Aufgrund der frühen Version des EF in Verbindung mit .NET Core ist dieses Arbeitpaket einzeln, da dort noch viele Fehlerquellen zu erwarten sind. (siehe: https://github.com/aspnet/EntityFramework.Docs/blob/master/docs/platforms/netcore/new-db-sqlite.rst)</t>
+  </si>
+  <si>
+    <t>Hier müssen die Routen implementiert werden, auf die das Frontend zugreift. Da das Team bisher keine Erfahrung mit einer REST-Api mit den zugrunde liegenden Technologie kann dieses Arbeitspaket nicht in kleinere Teile aufgeteilt werden.</t>
+  </si>
+  <si>
+    <t>Die Abschlusspräsentation muss erstellt werden. Format: PowerPoint</t>
+  </si>
+  <si>
+    <t>Die Abschlusspräsentation muss hier gehalten werden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -349,6 +421,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,7 +485,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -462,7 +537,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -656,29 +731,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="3" width="57.875" customWidth="1"/>
     <col min="6" max="6" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,367 +767,429 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="90">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="90">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="90">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="120">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="135">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="195">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="165">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="120">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="180">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="150">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="60">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="60">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="60">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="60">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="120">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="105">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="90">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="120">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="105">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1064,39 +1201,45 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="105">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1108,7 +1251,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1120,7 +1263,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1132,7 +1275,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1144,7 +1287,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
@@ -1156,7 +1299,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -1168,7 +1311,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
@@ -1180,7 +1323,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1192,7 +1335,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -1204,17 +1347,19 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -1226,61 +1371,71 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="45">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="135">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="3"/>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B52" s="3"/>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
         <v>43</v>
       </c>
@@ -1292,7 +1447,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -1304,7 +1459,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
         <v>44</v>
       </c>
@@ -1316,7 +1471,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -1328,7 +1483,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
         <v>46</v>
       </c>
@@ -1340,7 +1495,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
@@ -1352,7 +1507,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
         <v>47</v>
       </c>
@@ -1364,7 +1519,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -1376,7 +1531,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
         <v>48</v>
       </c>
@@ -1388,7 +1543,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -1400,7 +1555,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
         <v>49</v>
       </c>
@@ -1412,7 +1567,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -1424,7 +1579,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -1436,7 +1591,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -1448,7 +1603,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
         <v>41</v>
       </c>
@@ -1460,7 +1615,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
         <v>65</v>
       </c>
@@ -1472,7 +1627,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
         <v>42</v>
       </c>
@@ -1484,7 +1639,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
@@ -1496,43 +1651,58 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="45">
       <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C72" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="90">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C73" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="60">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
         <v>72</v>
       </c>
@@ -1540,33 +1710,45 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6">
       <c r="A77" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B80" s="3"/>
+      <c r="C80" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>